<commit_message>
Add units to output file for summary stats
</commit_message>
<xml_diff>
--- a/R_analysis/summary_stats/SSFA_summary-stats.xlsx
+++ b/R_analysis/summary_stats/SSFA_summary-stats.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="summary_stats" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="units" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -237,6 +238,51 @@
   </si>
   <si>
     <t xml:space="preserve">BrushDirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epLsar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;no unit&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NewEplsar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rsquared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asfc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smfc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">µm²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAsfc9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAsfc81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toothfrax_units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">µm</t>
   </si>
 </sst>
 </file>
@@ -7378,4 +7424,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate summary stats on all surfaces by NMP_cat
</commit_message>
<xml_diff>
--- a/R_analysis/summary_stats/SSFA_summary-stats.xlsx
+++ b/R_analysis/summary_stats/SSFA_summary-stats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t xml:space="preserve">Before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20-100%</t>
   </si>
   <si>
     <t xml:space="preserve">After</t>
@@ -4899,158 +4902,142 @@
         <v>69</v>
       </c>
       <c r="D28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" t="s">
         <v>71</v>
-      </c>
-      <c r="E28" t="s">
-        <v>56</v>
       </c>
       <c r="F28" t="s">
         <v>57</v>
       </c>
       <c r="G28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>0.2394835485</v>
+        <v>45.75842242</v>
       </c>
       <c r="I28" t="n">
-        <v>4.866895738</v>
+        <v>45.75842242</v>
       </c>
       <c r="J28" t="n">
-        <v>2.971779698375</v>
+        <v>45.75842242</v>
       </c>
       <c r="K28" t="n">
-        <v>3.3903697535</v>
-      </c>
-      <c r="L28" t="n">
-        <v>2.10587103778341</v>
-      </c>
+        <v>45.75842242</v>
+      </c>
+      <c r="L28"/>
       <c r="M28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N28" t="n">
-        <v>0.002003087339</v>
+        <v>0.002191890821</v>
       </c>
       <c r="O28" t="n">
-        <v>0.004004750868</v>
+        <v>0.002191890821</v>
       </c>
       <c r="P28" t="n">
-        <v>0.002851159634</v>
+        <v>0.002191890821</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.0026984001645</v>
-      </c>
-      <c r="R28" t="n">
-        <v>0.00083636224816724</v>
-      </c>
+        <v>0.002191890821</v>
+      </c>
+      <c r="R28"/>
       <c r="S28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T28" t="n">
-        <v>0.9934198948</v>
+        <v>0.9971472533</v>
       </c>
       <c r="U28" t="n">
-        <v>0.9991144199</v>
+        <v>0.9971472533</v>
       </c>
       <c r="V28" t="n">
-        <v>0.9973466185</v>
+        <v>0.9971472533</v>
       </c>
       <c r="W28" t="n">
-        <v>0.99842607965</v>
-      </c>
-      <c r="X28" t="n">
-        <v>0.00269480417669345</v>
-      </c>
+        <v>0.9971472533</v>
+      </c>
+      <c r="X28"/>
       <c r="Y28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z28" t="n">
-        <v>2.445318468</v>
+        <v>68.22224309</v>
       </c>
       <c r="AA28" t="n">
-        <v>49.1789018</v>
+        <v>68.22224309</v>
       </c>
       <c r="AB28" t="n">
-        <v>29.909897767</v>
+        <v>68.22224309</v>
       </c>
       <c r="AC28" t="n">
-        <v>34.0076854</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>21.5713496215021</v>
-      </c>
+        <v>68.22224309</v>
+      </c>
+      <c r="AD28"/>
       <c r="AE28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AF28" t="n">
-        <v>0.07838834353</v>
+        <v>0.3068635466</v>
       </c>
       <c r="AG28" t="n">
-        <v>0.2250309019</v>
+        <v>0.3068635466</v>
       </c>
       <c r="AH28" t="n">
-        <v>0.1260872200075</v>
+        <v>0.3068635466</v>
       </c>
       <c r="AI28" t="n">
-        <v>0.1004648173</v>
-      </c>
-      <c r="AJ28" t="n">
-        <v>0.066778364871343</v>
-      </c>
+        <v>0.3068635466</v>
+      </c>
+      <c r="AJ28"/>
       <c r="AK28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AL28" t="n">
-        <v>0.1753363325</v>
+        <v>0.1617157036</v>
       </c>
       <c r="AM28" t="n">
-        <v>0.7292764348</v>
+        <v>0.1617157036</v>
       </c>
       <c r="AN28" t="n">
-        <v>0.406228249725</v>
+        <v>0.1617157036</v>
       </c>
       <c r="AO28" t="n">
-        <v>0.3601501158</v>
-      </c>
-      <c r="AP28" t="n">
-        <v>0.259898151969492</v>
-      </c>
+        <v>0.1617157036</v>
+      </c>
+      <c r="AP28"/>
       <c r="AQ28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AR28" t="n">
-        <v>0.3175200085</v>
+        <v>0.2868278611</v>
       </c>
       <c r="AS28" t="n">
-        <v>1.478204278</v>
+        <v>0.2868278611</v>
       </c>
       <c r="AT28" t="n">
-        <v>0.90357104865</v>
+        <v>0.2868278611</v>
       </c>
       <c r="AU28" t="n">
-        <v>0.90927995405</v>
-      </c>
-      <c r="AV28" t="n">
-        <v>0.618889457066963</v>
-      </c>
+        <v>0.2868278611</v>
+      </c>
+      <c r="AV28"/>
       <c r="AW28" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AX28" t="n">
-        <v>0.01660217518</v>
+        <v>0.01710405668</v>
       </c>
       <c r="AY28" t="n">
-        <v>0.01869619765</v>
+        <v>0.01710405668</v>
       </c>
       <c r="AZ28" t="n">
-        <v>0.0179062071175</v>
+        <v>0.01710405668</v>
       </c>
       <c r="BA28" t="n">
-        <v>0.01816322782</v>
-      </c>
-      <c r="BB28" t="n">
-        <v>0.000938902161312765</v>
-      </c>
+        <v>0.01710405668</v>
+      </c>
+      <c r="BB28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -5061,140 +5048,126 @@
         <v>69</v>
       </c>
       <c r="D29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" t="s">
         <v>71</v>
-      </c>
-      <c r="E29" t="s">
-        <v>56</v>
       </c>
       <c r="F29" t="s">
         <v>58</v>
       </c>
       <c r="G29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>0.2394835485</v>
+        <v>45.75842242</v>
       </c>
       <c r="I29" t="n">
-        <v>4.866895738</v>
+        <v>45.75842242</v>
       </c>
       <c r="J29" t="n">
-        <v>2.971779698375</v>
+        <v>45.75842242</v>
       </c>
       <c r="K29" t="n">
-        <v>3.3903697535</v>
-      </c>
-      <c r="L29" t="n">
-        <v>2.10587103778341</v>
-      </c>
+        <v>45.75842242</v>
+      </c>
+      <c r="L29"/>
       <c r="M29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N29" t="n">
-        <v>0.001742</v>
+        <v>0.002427</v>
       </c>
       <c r="O29" t="n">
-        <v>0.004307</v>
+        <v>0.002427</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0029625</v>
+        <v>0.002427</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.0029005</v>
-      </c>
-      <c r="R29" t="n">
-        <v>0.00130584493719584</v>
-      </c>
+        <v>0.002427</v>
+      </c>
+      <c r="R29"/>
       <c r="S29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T29" t="n">
-        <v>0.999254</v>
+        <v>0.999645</v>
       </c>
       <c r="U29" t="n">
-        <v>0.999792</v>
+        <v>0.999645</v>
       </c>
       <c r="V29" t="n">
-        <v>0.999478</v>
+        <v>0.999645</v>
       </c>
       <c r="W29" t="n">
-        <v>0.999433</v>
-      </c>
-      <c r="X29" t="n">
-        <v>0.000228169527617829</v>
-      </c>
+        <v>0.999645</v>
+      </c>
+      <c r="X29"/>
       <c r="Y29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z29" t="n">
-        <v>2.314131</v>
+        <v>56.316945</v>
       </c>
       <c r="AA29" t="n">
-        <v>41.260755</v>
+        <v>56.316945</v>
       </c>
       <c r="AB29" t="n">
-        <v>25.23230975</v>
+        <v>56.316945</v>
       </c>
       <c r="AC29" t="n">
-        <v>28.6771765</v>
-      </c>
-      <c r="AD29" t="n">
-        <v>18.2972151098333</v>
-      </c>
+        <v>56.316945</v>
+      </c>
+      <c r="AD29"/>
       <c r="AE29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AF29" t="n">
-        <v>0.014514</v>
+        <v>0.058054</v>
       </c>
       <c r="AG29" t="n">
-        <v>0.09071</v>
+        <v>0.058054</v>
       </c>
       <c r="AH29" t="n">
-        <v>0.03809825</v>
+        <v>0.058054</v>
       </c>
       <c r="AI29" t="n">
-        <v>0.0235845</v>
-      </c>
-      <c r="AJ29" t="n">
-        <v>0.0361019801153621</v>
-      </c>
+        <v>0.058054</v>
+      </c>
+      <c r="AJ29"/>
       <c r="AK29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AL29" t="n">
-        <v>0.142359129935648</v>
+        <v>0.115188511626691</v>
       </c>
       <c r="AM29" t="n">
-        <v>0.627918961281224</v>
+        <v>0.115188511626691</v>
       </c>
       <c r="AN29" t="n">
-        <v>0.363768093949634</v>
+        <v>0.115188511626691</v>
       </c>
       <c r="AO29" t="n">
-        <v>0.342397142290832</v>
-      </c>
-      <c r="AP29" t="n">
-        <v>0.250867160114767</v>
-      </c>
+        <v>0.115188511626691</v>
+      </c>
+      <c r="AP29"/>
       <c r="AQ29" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AR29" t="n">
-        <v>0.238377296804313</v>
+        <v>0.213858546040502</v>
       </c>
       <c r="AS29" t="n">
-        <v>1.26792759112418</v>
+        <v>0.213858546040502</v>
       </c>
       <c r="AT29" t="n">
-        <v>0.773810634947521</v>
+        <v>0.213858546040502</v>
       </c>
       <c r="AU29" t="n">
-        <v>0.794468825930796</v>
-      </c>
-      <c r="AV29" t="n">
-        <v>0.545706120507354</v>
-      </c>
+        <v>0.213858546040502</v>
+      </c>
+      <c r="AV29"/>
       <c r="AW29" t="n">
         <v>0</v>
       </c>
@@ -5216,10 +5189,10 @@
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" t="s">
         <v>72</v>
-      </c>
-      <c r="D30" t="s">
-        <v>70</v>
       </c>
       <c r="E30" t="s">
         <v>56</v>
@@ -5231,145 +5204,145 @@
         <v>4</v>
       </c>
       <c r="H30" t="n">
-        <v>0.2889421075</v>
+        <v>0.2394835485</v>
       </c>
       <c r="I30" t="n">
-        <v>4.101011153</v>
+        <v>4.866895738</v>
       </c>
       <c r="J30" t="n">
-        <v>2.866861030125</v>
+        <v>2.971779698375</v>
       </c>
       <c r="K30" t="n">
-        <v>3.53874543</v>
+        <v>3.3903697535</v>
       </c>
       <c r="L30" t="n">
-        <v>1.77674843592688</v>
+        <v>2.10587103778341</v>
       </c>
       <c r="M30" t="n">
         <v>4</v>
       </c>
       <c r="N30" t="n">
-        <v>0.001557564455</v>
+        <v>0.002003087339</v>
       </c>
       <c r="O30" t="n">
-        <v>0.007075581839</v>
+        <v>0.004004750868</v>
       </c>
       <c r="P30" t="n">
-        <v>0.0039216402375</v>
+        <v>0.002851159634</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.003526707328</v>
+        <v>0.0026984001645</v>
       </c>
       <c r="R30" t="n">
-        <v>0.00259226232461313</v>
+        <v>0.00083636224816724</v>
       </c>
       <c r="S30" t="n">
         <v>4</v>
       </c>
       <c r="T30" t="n">
-        <v>0.9233653816</v>
+        <v>0.9934198948</v>
       </c>
       <c r="U30" t="n">
-        <v>0.9981923748</v>
+        <v>0.9991144199</v>
       </c>
       <c r="V30" t="n">
-        <v>0.97551618815</v>
+        <v>0.9973466185</v>
       </c>
       <c r="W30" t="n">
-        <v>0.9902534981</v>
+        <v>0.99842607965</v>
       </c>
       <c r="X30" t="n">
-        <v>0.0354806249349532</v>
+        <v>0.00269480417669345</v>
       </c>
       <c r="Y30" t="n">
         <v>4</v>
       </c>
       <c r="Z30" t="n">
-        <v>1.6949705</v>
+        <v>2.445318468</v>
       </c>
       <c r="AA30" t="n">
-        <v>55.58561369</v>
+        <v>49.1789018</v>
       </c>
       <c r="AB30" t="n">
-        <v>30.559207425</v>
+        <v>29.909897767</v>
       </c>
       <c r="AC30" t="n">
-        <v>32.478122755</v>
+        <v>34.0076854</v>
       </c>
       <c r="AD30" t="n">
-        <v>28.2912120795614</v>
+        <v>21.5713496215021</v>
       </c>
       <c r="AE30" t="n">
         <v>4</v>
       </c>
       <c r="AF30" t="n">
-        <v>0.08340500545</v>
+        <v>0.07838834353</v>
       </c>
       <c r="AG30" t="n">
-        <v>0.9972802751</v>
+        <v>0.2250309019</v>
       </c>
       <c r="AH30" t="n">
-        <v>0.3204037287875</v>
+        <v>0.1260872200075</v>
       </c>
       <c r="AI30" t="n">
         <v>0.1004648173</v>
       </c>
       <c r="AJ30" t="n">
-        <v>0.451322686993152</v>
+        <v>0.066778364871343</v>
       </c>
       <c r="AK30" t="n">
         <v>4</v>
       </c>
       <c r="AL30" t="n">
-        <v>0.1004931439</v>
+        <v>0.1753363325</v>
       </c>
       <c r="AM30" t="n">
-        <v>10.32469331</v>
+        <v>0.7292764348</v>
       </c>
       <c r="AN30" t="n">
-        <v>2.8761120663</v>
+        <v>0.406228249725</v>
       </c>
       <c r="AO30" t="n">
-        <v>0.53963090565</v>
+        <v>0.3601501158</v>
       </c>
       <c r="AP30" t="n">
-        <v>4.98238226572338</v>
+        <v>0.259898151969492</v>
       </c>
       <c r="AQ30" t="n">
         <v>4</v>
       </c>
       <c r="AR30" t="n">
-        <v>0.1951037382</v>
+        <v>0.3175200085</v>
       </c>
       <c r="AS30" t="n">
-        <v>36.41591664</v>
+        <v>1.478204278</v>
       </c>
       <c r="AT30" t="n">
-        <v>10.658599809125</v>
+        <v>0.90357104865</v>
       </c>
       <c r="AU30" t="n">
-        <v>3.01168942915</v>
+        <v>0.90927995405</v>
       </c>
       <c r="AV30" t="n">
-        <v>17.3721702577839</v>
+        <v>0.618889457066963</v>
       </c>
       <c r="AW30" t="n">
         <v>4</v>
       </c>
       <c r="AX30" t="n">
-        <v>0.01649338863</v>
+        <v>0.01660217518</v>
       </c>
       <c r="AY30" t="n">
-        <v>0.01795356794</v>
+        <v>0.01869619765</v>
       </c>
       <c r="AZ30" t="n">
-        <v>0.0170521764775</v>
+        <v>0.0179062071175</v>
       </c>
       <c r="BA30" t="n">
-        <v>0.01688087467</v>
+        <v>0.01816322782</v>
       </c>
       <c r="BB30" t="n">
-        <v>0.000637577056355895</v>
+        <v>0.000938902161312765</v>
       </c>
     </row>
     <row r="31">
@@ -5378,10 +5351,10 @@
       </c>
       <c r="B31"/>
       <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" t="s">
         <v>72</v>
-      </c>
-      <c r="D31" t="s">
-        <v>70</v>
       </c>
       <c r="E31" t="s">
         <v>56</v>
@@ -5393,73 +5366,73 @@
         <v>4</v>
       </c>
       <c r="H31" t="n">
-        <v>0.2889421075</v>
+        <v>0.2394835485</v>
       </c>
       <c r="I31" t="n">
-        <v>4.101011153</v>
+        <v>4.866895738</v>
       </c>
       <c r="J31" t="n">
-        <v>2.866861030125</v>
+        <v>2.971779698375</v>
       </c>
       <c r="K31" t="n">
-        <v>3.53874543</v>
+        <v>3.3903697535</v>
       </c>
       <c r="L31" t="n">
-        <v>1.77674843592688</v>
+        <v>2.10587103778341</v>
       </c>
       <c r="M31" t="n">
         <v>4</v>
       </c>
       <c r="N31" t="n">
-        <v>0.001734</v>
+        <v>0.001742</v>
       </c>
       <c r="O31" t="n">
-        <v>0.009166</v>
+        <v>0.004307</v>
       </c>
       <c r="P31" t="n">
-        <v>0.00373875</v>
+        <v>0.0029625</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.0020275</v>
+        <v>0.0029005</v>
       </c>
       <c r="R31" t="n">
-        <v>0.00362195539959656</v>
+        <v>0.00130584493719584</v>
       </c>
       <c r="S31" t="n">
         <v>4</v>
       </c>
       <c r="T31" t="n">
-        <v>0.996661</v>
+        <v>0.999254</v>
       </c>
       <c r="U31" t="n">
-        <v>0.999563</v>
+        <v>0.999792</v>
       </c>
       <c r="V31" t="n">
-        <v>0.998579</v>
+        <v>0.999478</v>
       </c>
       <c r="W31" t="n">
-        <v>0.999046</v>
+        <v>0.999433</v>
       </c>
       <c r="X31" t="n">
-        <v>0.00134756768537487</v>
+        <v>0.000228169527617829</v>
       </c>
       <c r="Y31" t="n">
         <v>4</v>
       </c>
       <c r="Z31" t="n">
-        <v>1.453198</v>
+        <v>2.314131</v>
       </c>
       <c r="AA31" t="n">
-        <v>47.532028</v>
+        <v>41.260755</v>
       </c>
       <c r="AB31" t="n">
-        <v>26.59509575</v>
+        <v>25.23230975</v>
       </c>
       <c r="AC31" t="n">
-        <v>28.6975785</v>
+        <v>28.6771765</v>
       </c>
       <c r="AD31" t="n">
-        <v>23.5756902381135</v>
+        <v>18.2972151098333</v>
       </c>
       <c r="AE31" t="n">
         <v>4</v>
@@ -5468,52 +5441,52 @@
         <v>0.014514</v>
       </c>
       <c r="AG31" t="n">
-        <v>0.928866</v>
+        <v>0.09071</v>
       </c>
       <c r="AH31" t="n">
-        <v>0.24763725</v>
+        <v>0.03809825</v>
       </c>
       <c r="AI31" t="n">
         <v>0.0235845</v>
       </c>
       <c r="AJ31" t="n">
-        <v>0.454233008129363</v>
+        <v>0.0361019801153621</v>
       </c>
       <c r="AK31" t="n">
         <v>4</v>
       </c>
       <c r="AL31" t="n">
-        <v>0.0735873258428672</v>
+        <v>0.142359129935648</v>
       </c>
       <c r="AM31" t="n">
-        <v>3.63859440283608</v>
+        <v>0.627918961281224</v>
       </c>
       <c r="AN31" t="n">
-        <v>1.2589910647095</v>
+        <v>0.363768093949634</v>
       </c>
       <c r="AO31" t="n">
-        <v>0.661891265079533</v>
+        <v>0.342397142290832</v>
       </c>
       <c r="AP31" t="n">
-        <v>1.67813712666212</v>
+        <v>0.250867160114767</v>
       </c>
       <c r="AQ31" t="n">
         <v>4</v>
       </c>
       <c r="AR31" t="n">
-        <v>0.139404927919054</v>
+        <v>0.238377296804313</v>
       </c>
       <c r="AS31" t="n">
-        <v>6.98551143117234</v>
+        <v>1.26792759112418</v>
       </c>
       <c r="AT31" t="n">
-        <v>2.72493695381651</v>
+        <v>0.773810634947521</v>
       </c>
       <c r="AU31" t="n">
-        <v>1.88741572808731</v>
+        <v>0.794468825930796</v>
       </c>
       <c r="AV31" t="n">
-        <v>3.27735427973907</v>
+        <v>0.545706120507354</v>
       </c>
       <c r="AW31" t="n">
         <v>0</v>
@@ -5536,10 +5509,10 @@
       </c>
       <c r="B32"/>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
         <v>56</v>
@@ -5551,145 +5524,145 @@
         <v>4</v>
       </c>
       <c r="H32" t="n">
-        <v>0.2736128465</v>
+        <v>0.2889421075</v>
       </c>
       <c r="I32" t="n">
-        <v>4.661541487</v>
+        <v>4.101011153</v>
       </c>
       <c r="J32" t="n">
-        <v>2.737068466625</v>
+        <v>2.866861030125</v>
       </c>
       <c r="K32" t="n">
-        <v>3.0065597665</v>
+        <v>3.53874543</v>
       </c>
       <c r="L32" t="n">
-        <v>2.16436934525046</v>
+        <v>1.77674843592688</v>
       </c>
       <c r="M32" t="n">
         <v>4</v>
       </c>
       <c r="N32" t="n">
-        <v>0.0003305038118</v>
+        <v>0.001557564455</v>
       </c>
       <c r="O32" t="n">
-        <v>0.006599490184</v>
+        <v>0.007075581839</v>
       </c>
       <c r="P32" t="n">
-        <v>0.0039659883497</v>
+        <v>0.0039216402375</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.0044669797015</v>
+        <v>0.003526707328</v>
       </c>
       <c r="R32" t="n">
-        <v>0.0028839563689639</v>
+        <v>0.00259226232461313</v>
       </c>
       <c r="S32" t="n">
         <v>4</v>
       </c>
       <c r="T32" t="n">
-        <v>0.9097145607</v>
+        <v>0.9233653816</v>
       </c>
       <c r="U32" t="n">
-        <v>0.9988839764</v>
+        <v>0.9981923748</v>
       </c>
       <c r="V32" t="n">
-        <v>0.975850219425</v>
+        <v>0.97551618815</v>
       </c>
       <c r="W32" t="n">
-        <v>0.9974011703</v>
+        <v>0.9902534981</v>
       </c>
       <c r="X32" t="n">
-        <v>0.0441035891856082</v>
+        <v>0.0354806249349532</v>
       </c>
       <c r="Y32" t="n">
         <v>4</v>
       </c>
       <c r="Z32" t="n">
-        <v>4.197067473</v>
+        <v>1.6949705</v>
       </c>
       <c r="AA32" t="n">
-        <v>52.04521745</v>
+        <v>55.58561369</v>
       </c>
       <c r="AB32" t="n">
-        <v>22.60779744275</v>
+        <v>30.559207425</v>
       </c>
       <c r="AC32" t="n">
-        <v>17.094452424</v>
+        <v>32.478122755</v>
       </c>
       <c r="AD32" t="n">
-        <v>22.8685932726795</v>
+        <v>28.2912120795614</v>
       </c>
       <c r="AE32" t="n">
         <v>4</v>
       </c>
       <c r="AF32" t="n">
-        <v>0.07838834353</v>
+        <v>0.08340500545</v>
       </c>
       <c r="AG32" t="n">
-        <v>3.04613068</v>
+        <v>0.9972802751</v>
       </c>
       <c r="AH32" t="n">
-        <v>0.8501414256075</v>
+        <v>0.3204037287875</v>
       </c>
       <c r="AI32" t="n">
-        <v>0.13802333945</v>
+        <v>0.1004648173</v>
       </c>
       <c r="AJ32" t="n">
-        <v>1.46458381432416</v>
+        <v>0.451322686993152</v>
       </c>
       <c r="AK32" t="n">
         <v>4</v>
       </c>
       <c r="AL32" t="n">
-        <v>0.160685842</v>
+        <v>0.1004931439</v>
       </c>
       <c r="AM32" t="n">
-        <v>5.640511661</v>
+        <v>10.32469331</v>
       </c>
       <c r="AN32" t="n">
-        <v>2.072835025425</v>
+        <v>2.8761120663</v>
       </c>
       <c r="AO32" t="n">
-        <v>1.24507129935</v>
+        <v>0.53963090565</v>
       </c>
       <c r="AP32" t="n">
-        <v>2.56337421790091</v>
+        <v>4.98238226572338</v>
       </c>
       <c r="AQ32" t="n">
         <v>4</v>
       </c>
       <c r="AR32" t="n">
-        <v>0.2179132886</v>
+        <v>0.1951037382</v>
       </c>
       <c r="AS32" t="n">
-        <v>10.21086867</v>
+        <v>36.41591664</v>
       </c>
       <c r="AT32" t="n">
-        <v>3.33805785855</v>
+        <v>10.658599809125</v>
       </c>
       <c r="AU32" t="n">
-        <v>1.4617247378</v>
+        <v>3.01168942915</v>
       </c>
       <c r="AV32" t="n">
-        <v>4.67001566513468</v>
+        <v>17.3721702577839</v>
       </c>
       <c r="AW32" t="n">
         <v>4</v>
       </c>
       <c r="AX32" t="n">
-        <v>0.01595719018</v>
+        <v>0.01649338863</v>
       </c>
       <c r="AY32" t="n">
-        <v>0.01888923869</v>
+        <v>0.01795356794</v>
       </c>
       <c r="AZ32" t="n">
-        <v>0.01732885529</v>
+        <v>0.0170521764775</v>
       </c>
       <c r="BA32" t="n">
-        <v>0.017234496145</v>
+        <v>0.01688087467</v>
       </c>
       <c r="BB32" t="n">
-        <v>0.00125497658850918</v>
+        <v>0.000637577056355895</v>
       </c>
     </row>
     <row r="33">
@@ -5698,10 +5671,10 @@
       </c>
       <c r="B33"/>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
         <v>56</v>
@@ -5713,73 +5686,73 @@
         <v>4</v>
       </c>
       <c r="H33" t="n">
-        <v>0.2736128465</v>
+        <v>0.2889421075</v>
       </c>
       <c r="I33" t="n">
-        <v>4.661541487</v>
+        <v>4.101011153</v>
       </c>
       <c r="J33" t="n">
-        <v>2.737068466625</v>
+        <v>2.866861030125</v>
       </c>
       <c r="K33" t="n">
-        <v>3.0065597665</v>
+        <v>3.53874543</v>
       </c>
       <c r="L33" t="n">
-        <v>2.16436934525046</v>
+        <v>1.77674843592688</v>
       </c>
       <c r="M33" t="n">
         <v>4</v>
       </c>
       <c r="N33" t="n">
-        <v>0.000644</v>
+        <v>0.001734</v>
       </c>
       <c r="O33" t="n">
-        <v>0.009006</v>
+        <v>0.009166</v>
       </c>
       <c r="P33" t="n">
-        <v>0.00369</v>
+        <v>0.00373875</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.002555</v>
+        <v>0.0020275</v>
       </c>
       <c r="R33" t="n">
-        <v>0.00366152163269134</v>
+        <v>0.00362195539959656</v>
       </c>
       <c r="S33" t="n">
         <v>4</v>
       </c>
       <c r="T33" t="n">
-        <v>0.99525</v>
+        <v>0.996661</v>
       </c>
       <c r="U33" t="n">
-        <v>0.999789</v>
+        <v>0.999563</v>
       </c>
       <c r="V33" t="n">
-        <v>0.9982295</v>
+        <v>0.998579</v>
       </c>
       <c r="W33" t="n">
-        <v>0.9989395</v>
+        <v>0.999046</v>
       </c>
       <c r="X33" t="n">
-        <v>0.00202812894067416</v>
+        <v>0.00134756768537487</v>
       </c>
       <c r="Y33" t="n">
         <v>4</v>
       </c>
       <c r="Z33" t="n">
-        <v>3.616868</v>
+        <v>1.453198</v>
       </c>
       <c r="AA33" t="n">
-        <v>44.129257</v>
+        <v>47.532028</v>
       </c>
       <c r="AB33" t="n">
-        <v>19.60592075</v>
+        <v>26.59509575</v>
       </c>
       <c r="AC33" t="n">
-        <v>15.338779</v>
+        <v>28.6975785</v>
       </c>
       <c r="AD33" t="n">
-        <v>19.2327629261984</v>
+        <v>23.5756902381135</v>
       </c>
       <c r="AE33" t="n">
         <v>4</v>
@@ -5791,49 +5764,49 @@
         <v>0.928866</v>
       </c>
       <c r="AH33" t="n">
-        <v>0.26668625</v>
+        <v>0.24763725</v>
       </c>
       <c r="AI33" t="n">
-        <v>0.0616825</v>
+        <v>0.0235845</v>
       </c>
       <c r="AJ33" t="n">
-        <v>0.442647764978261</v>
+        <v>0.454233008129363</v>
       </c>
       <c r="AK33" t="n">
         <v>4</v>
       </c>
       <c r="AL33" t="n">
-        <v>0.103363088185532</v>
+        <v>0.0735873258428672</v>
       </c>
       <c r="AM33" t="n">
-        <v>3.07404466664286</v>
+        <v>3.63859440283608</v>
       </c>
       <c r="AN33" t="n">
-        <v>1.48085541219035</v>
+        <v>1.2589910647095</v>
       </c>
       <c r="AO33" t="n">
-        <v>1.3730069469665</v>
+        <v>0.661891265079533</v>
       </c>
       <c r="AP33" t="n">
-        <v>1.5149265269514</v>
+        <v>1.67813712666212</v>
       </c>
       <c r="AQ33" t="n">
         <v>4</v>
       </c>
       <c r="AR33" t="n">
-        <v>0.158442470474773</v>
+        <v>0.139404927919054</v>
       </c>
       <c r="AS33" t="n">
-        <v>4.34188139028749</v>
+        <v>6.98551143117234</v>
       </c>
       <c r="AT33" t="n">
-        <v>1.91442049832525</v>
+        <v>2.72493695381651</v>
       </c>
       <c r="AU33" t="n">
-        <v>1.57867906626938</v>
+        <v>1.88741572808731</v>
       </c>
       <c r="AV33" t="n">
-        <v>1.92128876439113</v>
+        <v>3.27735427973907</v>
       </c>
       <c r="AW33" t="n">
         <v>0</v>
@@ -5859,7 +5832,7 @@
         <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
         <v>56</v>
@@ -5871,145 +5844,145 @@
         <v>4</v>
       </c>
       <c r="H34" t="n">
-        <v>2.646177519</v>
+        <v>0.2736128465</v>
       </c>
       <c r="I34" t="n">
-        <v>4.923874312</v>
+        <v>4.661541487</v>
       </c>
       <c r="J34" t="n">
-        <v>3.97121858975</v>
+        <v>2.737068466625</v>
       </c>
       <c r="K34" t="n">
-        <v>4.157411264</v>
+        <v>3.0065597665</v>
       </c>
       <c r="L34" t="n">
-        <v>0.988439524190275</v>
+        <v>2.16436934525046</v>
       </c>
       <c r="M34" t="n">
         <v>4</v>
       </c>
       <c r="N34" t="n">
-        <v>0.001342898516</v>
+        <v>0.0003305038118</v>
       </c>
       <c r="O34" t="n">
-        <v>0.005991581983</v>
+        <v>0.006599490184</v>
       </c>
       <c r="P34" t="n">
-        <v>0.00356916864575</v>
+        <v>0.0039659883497</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.003471097042</v>
+        <v>0.0044669797015</v>
       </c>
       <c r="R34" t="n">
-        <v>0.00218887888416554</v>
+        <v>0.0028839563689639</v>
       </c>
       <c r="S34" t="n">
         <v>4</v>
       </c>
       <c r="T34" t="n">
-        <v>0.9935653584</v>
+        <v>0.9097145607</v>
       </c>
       <c r="U34" t="n">
-        <v>0.9988323968</v>
+        <v>0.9988839764</v>
       </c>
       <c r="V34" t="n">
-        <v>0.997009441725</v>
+        <v>0.975850219425</v>
       </c>
       <c r="W34" t="n">
-        <v>0.99782000585</v>
+        <v>0.9974011703</v>
       </c>
       <c r="X34" t="n">
-        <v>0.00240439309929278</v>
+        <v>0.0441035891856082</v>
       </c>
       <c r="Y34" t="n">
         <v>4</v>
       </c>
       <c r="Z34" t="n">
-        <v>29.63050783</v>
+        <v>4.197067473</v>
       </c>
       <c r="AA34" t="n">
-        <v>44.85846689</v>
+        <v>52.04521745</v>
       </c>
       <c r="AB34" t="n">
-        <v>36.36487685</v>
+        <v>22.60779744275</v>
       </c>
       <c r="AC34" t="n">
-        <v>35.48526634</v>
+        <v>17.094452424</v>
       </c>
       <c r="AD34" t="n">
-        <v>6.78599069455892</v>
+        <v>22.8685932726795</v>
       </c>
       <c r="AE34" t="n">
         <v>4</v>
       </c>
       <c r="AF34" t="n">
-        <v>0.1004648173</v>
+        <v>0.07838834353</v>
       </c>
       <c r="AG34" t="n">
-        <v>0.3265020617</v>
+        <v>3.04613068</v>
       </c>
       <c r="AH34" t="n">
-        <v>0.17311315575</v>
+        <v>0.8501414256075</v>
       </c>
       <c r="AI34" t="n">
-        <v>0.132742872</v>
+        <v>0.13802333945</v>
       </c>
       <c r="AJ34" t="n">
-        <v>0.106691459824779</v>
+        <v>1.46458381432416</v>
       </c>
       <c r="AK34" t="n">
         <v>4</v>
       </c>
       <c r="AL34" t="n">
-        <v>0.09025540084</v>
+        <v>0.160685842</v>
       </c>
       <c r="AM34" t="n">
-        <v>1.729337224</v>
+        <v>5.640511661</v>
       </c>
       <c r="AN34" t="n">
-        <v>0.81853750061</v>
+        <v>2.072835025425</v>
       </c>
       <c r="AO34" t="n">
-        <v>0.7272786888</v>
+        <v>1.24507129935</v>
       </c>
       <c r="AP34" t="n">
-        <v>0.780064136384275</v>
+        <v>2.56337421790091</v>
       </c>
       <c r="AQ34" t="n">
         <v>4</v>
       </c>
       <c r="AR34" t="n">
-        <v>0.2586428146</v>
+        <v>0.2179132886</v>
       </c>
       <c r="AS34" t="n">
-        <v>5.076058089</v>
+        <v>10.21086867</v>
       </c>
       <c r="AT34" t="n">
-        <v>1.8595322501</v>
+        <v>3.33805785855</v>
       </c>
       <c r="AU34" t="n">
-        <v>1.0517140484</v>
+        <v>1.4617247378</v>
       </c>
       <c r="AV34" t="n">
-        <v>2.24785217127257</v>
+        <v>4.67001566513468</v>
       </c>
       <c r="AW34" t="n">
         <v>4</v>
       </c>
       <c r="AX34" t="n">
-        <v>0.01708514642</v>
+        <v>0.01595719018</v>
       </c>
       <c r="AY34" t="n">
-        <v>0.01764294591</v>
+        <v>0.01888923869</v>
       </c>
       <c r="AZ34" t="n">
-        <v>0.0173270408825</v>
+        <v>0.01732885529</v>
       </c>
       <c r="BA34" t="n">
-        <v>0.0172900356</v>
+        <v>0.017234496145</v>
       </c>
       <c r="BB34" t="n">
-        <v>0.000255857898743912</v>
+        <v>0.00125497658850918</v>
       </c>
     </row>
     <row r="35">
@@ -6021,7 +5994,7 @@
         <v>73</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
         <v>56</v>
@@ -6033,73 +6006,73 @@
         <v>4</v>
       </c>
       <c r="H35" t="n">
-        <v>2.646177519</v>
+        <v>0.2736128465</v>
       </c>
       <c r="I35" t="n">
-        <v>4.923874312</v>
+        <v>4.661541487</v>
       </c>
       <c r="J35" t="n">
-        <v>3.97121858975</v>
+        <v>2.737068466625</v>
       </c>
       <c r="K35" t="n">
-        <v>4.157411264</v>
+        <v>3.0065597665</v>
       </c>
       <c r="L35" t="n">
-        <v>0.988439524190275</v>
+        <v>2.16436934525046</v>
       </c>
       <c r="M35" t="n">
         <v>4</v>
       </c>
       <c r="N35" t="n">
-        <v>0.001843</v>
+        <v>0.000644</v>
       </c>
       <c r="O35" t="n">
-        <v>0.002678</v>
+        <v>0.009006</v>
       </c>
       <c r="P35" t="n">
-        <v>0.0021015</v>
+        <v>0.00369</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.0019425</v>
+        <v>0.002555</v>
       </c>
       <c r="R35" t="n">
-        <v>0.000394482361244876</v>
+        <v>0.00366152163269134</v>
       </c>
       <c r="S35" t="n">
         <v>4</v>
       </c>
       <c r="T35" t="n">
-        <v>0.99893</v>
+        <v>0.99525</v>
       </c>
       <c r="U35" t="n">
-        <v>0.999603</v>
+        <v>0.999789</v>
       </c>
       <c r="V35" t="n">
-        <v>0.99927075</v>
+        <v>0.9982295</v>
       </c>
       <c r="W35" t="n">
-        <v>0.999275</v>
+        <v>0.9989395</v>
       </c>
       <c r="X35" t="n">
-        <v>0.000364878404403459</v>
+        <v>0.00202812894067416</v>
       </c>
       <c r="Y35" t="n">
         <v>4</v>
       </c>
       <c r="Z35" t="n">
-        <v>23.258608</v>
+        <v>3.616868</v>
       </c>
       <c r="AA35" t="n">
-        <v>38.331227</v>
+        <v>44.129257</v>
       </c>
       <c r="AB35" t="n">
-        <v>29.811954</v>
+        <v>19.60592075</v>
       </c>
       <c r="AC35" t="n">
-        <v>28.8289905</v>
+        <v>15.338779</v>
       </c>
       <c r="AD35" t="n">
-        <v>6.56284659651471</v>
+        <v>19.2327629261984</v>
       </c>
       <c r="AE35" t="n">
         <v>4</v>
@@ -6108,52 +6081,52 @@
         <v>0.014514</v>
       </c>
       <c r="AG35" t="n">
-        <v>0.09071</v>
+        <v>0.928866</v>
       </c>
       <c r="AH35" t="n">
-        <v>0.044448</v>
+        <v>0.26668625</v>
       </c>
       <c r="AI35" t="n">
-        <v>0.036284</v>
+        <v>0.0616825</v>
       </c>
       <c r="AJ35" t="n">
-        <v>0.0370467479094544</v>
+        <v>0.442647764978261</v>
       </c>
       <c r="AK35" t="n">
         <v>4</v>
       </c>
       <c r="AL35" t="n">
-        <v>0.0808756703113495</v>
+        <v>0.103363088185532</v>
       </c>
       <c r="AM35" t="n">
-        <v>1.15120732776973</v>
+        <v>3.07404466664286</v>
       </c>
       <c r="AN35" t="n">
-        <v>0.611734478996843</v>
+        <v>1.48085541219035</v>
       </c>
       <c r="AO35" t="n">
-        <v>0.607427458953147</v>
+        <v>1.3730069469665</v>
       </c>
       <c r="AP35" t="n">
-        <v>0.548302195244949</v>
+        <v>1.5149265269514</v>
       </c>
       <c r="AQ35" t="n">
         <v>4</v>
       </c>
       <c r="AR35" t="n">
-        <v>0.214061442351137</v>
+        <v>0.158442470474773</v>
       </c>
       <c r="AS35" t="n">
-        <v>2.25215131553443</v>
+        <v>4.34188139028749</v>
       </c>
       <c r="AT35" t="n">
-        <v>1.06061524543021</v>
+        <v>1.91442049832525</v>
       </c>
       <c r="AU35" t="n">
-        <v>0.888124111917628</v>
+        <v>1.57867906626938</v>
       </c>
       <c r="AV35" t="n">
-        <v>0.976836337978275</v>
+        <v>1.92128876439113</v>
       </c>
       <c r="AW35" t="n">
         <v>0</v>
@@ -6176,10 +6149,10 @@
       </c>
       <c r="B36"/>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E36" t="s">
         <v>56</v>
@@ -6191,73 +6164,73 @@
         <v>4</v>
       </c>
       <c r="H36" t="n">
-        <v>0.3271206442</v>
+        <v>2.646177519</v>
       </c>
       <c r="I36" t="n">
-        <v>4.891769633</v>
+        <v>4.923874312</v>
       </c>
       <c r="J36" t="n">
-        <v>2.56107119705</v>
+        <v>3.97121858975</v>
       </c>
       <c r="K36" t="n">
-        <v>2.5126972555</v>
+        <v>4.157411264</v>
       </c>
       <c r="L36" t="n">
-        <v>1.9704067798324</v>
+        <v>0.988439524190275</v>
       </c>
       <c r="M36" t="n">
         <v>4</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0002049663924</v>
+        <v>0.001342898516</v>
       </c>
       <c r="O36" t="n">
-        <v>0.006006712705</v>
+        <v>0.005991581983</v>
       </c>
       <c r="P36" t="n">
-        <v>0.00304728943185</v>
+        <v>0.00356916864575</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.002988739315</v>
+        <v>0.003471097042</v>
       </c>
       <c r="R36" t="n">
-        <v>0.00255474362105596</v>
+        <v>0.00218887888416554</v>
       </c>
       <c r="S36" t="n">
         <v>4</v>
       </c>
       <c r="T36" t="n">
-        <v>0.987344213</v>
+        <v>0.9935653584</v>
       </c>
       <c r="U36" t="n">
-        <v>0.9985162009</v>
+        <v>0.9988323968</v>
       </c>
       <c r="V36" t="n">
-        <v>0.99477804315</v>
+        <v>0.997009441725</v>
       </c>
       <c r="W36" t="n">
-        <v>0.99662587935</v>
+        <v>0.99782000585</v>
       </c>
       <c r="X36" t="n">
-        <v>0.0052561963832895</v>
+        <v>0.00240439309929278</v>
       </c>
       <c r="Y36" t="n">
         <v>4</v>
       </c>
       <c r="Z36" t="n">
-        <v>5.671158448</v>
+        <v>29.63050783</v>
       </c>
       <c r="AA36" t="n">
-        <v>52.35611571</v>
+        <v>44.85846689</v>
       </c>
       <c r="AB36" t="n">
-        <v>28.93355824175</v>
+        <v>36.36487685</v>
       </c>
       <c r="AC36" t="n">
-        <v>28.8534794045</v>
+        <v>35.48526634</v>
       </c>
       <c r="AD36" t="n">
-        <v>24.7612557834655</v>
+        <v>6.78599069455892</v>
       </c>
       <c r="AE36" t="n">
         <v>4</v>
@@ -6266,70 +6239,70 @@
         <v>0.1004648173</v>
       </c>
       <c r="AG36" t="n">
-        <v>9.899664123</v>
+        <v>0.3265020617</v>
       </c>
       <c r="AH36" t="n">
-        <v>3.0500100059</v>
+        <v>0.17311315575</v>
       </c>
       <c r="AI36" t="n">
-        <v>1.09995554165</v>
+        <v>0.132742872</v>
       </c>
       <c r="AJ36" t="n">
-        <v>4.66265184155628</v>
+        <v>0.106691459824779</v>
       </c>
       <c r="AK36" t="n">
         <v>4</v>
       </c>
       <c r="AL36" t="n">
-        <v>0.145071985</v>
+        <v>0.09025540084</v>
       </c>
       <c r="AM36" t="n">
-        <v>0.8618896844</v>
+        <v>1.729337224</v>
       </c>
       <c r="AN36" t="n">
-        <v>0.4801019824</v>
+        <v>0.81853750061</v>
       </c>
       <c r="AO36" t="n">
-        <v>0.4567231301</v>
+        <v>0.7272786888</v>
       </c>
       <c r="AP36" t="n">
-        <v>0.384057841287175</v>
+        <v>0.780064136384275</v>
       </c>
       <c r="AQ36" t="n">
         <v>4</v>
       </c>
       <c r="AR36" t="n">
-        <v>0.2414260519</v>
+        <v>0.2586428146</v>
       </c>
       <c r="AS36" t="n">
-        <v>3.567648922</v>
+        <v>5.076058089</v>
       </c>
       <c r="AT36" t="n">
-        <v>1.41844556955</v>
+        <v>1.8595322501</v>
       </c>
       <c r="AU36" t="n">
-        <v>0.93235365215</v>
+        <v>1.0517140484</v>
       </c>
       <c r="AV36" t="n">
-        <v>1.56491684526697</v>
+        <v>2.24785217127257</v>
       </c>
       <c r="AW36" t="n">
         <v>4</v>
       </c>
       <c r="AX36" t="n">
-        <v>0.01698677161</v>
+        <v>0.01708514642</v>
       </c>
       <c r="AY36" t="n">
-        <v>0.02010935307</v>
+        <v>0.01764294591</v>
       </c>
       <c r="AZ36" t="n">
-        <v>0.01852792121</v>
+        <v>0.0173270408825</v>
       </c>
       <c r="BA36" t="n">
-        <v>0.01850778008</v>
+        <v>0.0172900356</v>
       </c>
       <c r="BB36" t="n">
-        <v>0.00145825624227347</v>
+        <v>0.000255857898743912</v>
       </c>
     </row>
     <row r="37">
@@ -6338,10 +6311,10 @@
       </c>
       <c r="B37"/>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
         <v>56</v>
@@ -6353,73 +6326,73 @@
         <v>4</v>
       </c>
       <c r="H37" t="n">
-        <v>0.3271206442</v>
+        <v>2.646177519</v>
       </c>
       <c r="I37" t="n">
-        <v>4.891769633</v>
+        <v>4.923874312</v>
       </c>
       <c r="J37" t="n">
-        <v>2.56107119705</v>
+        <v>3.97121858975</v>
       </c>
       <c r="K37" t="n">
-        <v>2.5126972555</v>
+        <v>4.157411264</v>
       </c>
       <c r="L37" t="n">
-        <v>1.9704067798324</v>
+        <v>0.988439524190275</v>
       </c>
       <c r="M37" t="n">
         <v>4</v>
       </c>
       <c r="N37" t="n">
-        <v>0.000446</v>
+        <v>0.001843</v>
       </c>
       <c r="O37" t="n">
-        <v>0.005429</v>
+        <v>0.002678</v>
       </c>
       <c r="P37" t="n">
-        <v>0.00289075</v>
+        <v>0.0021015</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.002844</v>
+        <v>0.0019425</v>
       </c>
       <c r="R37" t="n">
-        <v>0.00226717436103475</v>
+        <v>0.000394482361244876</v>
       </c>
       <c r="S37" t="n">
         <v>4</v>
       </c>
       <c r="T37" t="n">
-        <v>0.995536</v>
+        <v>0.99893</v>
       </c>
       <c r="U37" t="n">
-        <v>0.999635</v>
+        <v>0.999603</v>
       </c>
       <c r="V37" t="n">
-        <v>0.99752775</v>
+        <v>0.99927075</v>
       </c>
       <c r="W37" t="n">
-        <v>0.99747</v>
+        <v>0.999275</v>
       </c>
       <c r="X37" t="n">
-        <v>0.00215654297043519</v>
+        <v>0.000364878404403459</v>
       </c>
       <c r="Y37" t="n">
         <v>4</v>
       </c>
       <c r="Z37" t="n">
-        <v>5.658399</v>
+        <v>23.258608</v>
       </c>
       <c r="AA37" t="n">
-        <v>44.994782</v>
+        <v>38.331227</v>
       </c>
       <c r="AB37" t="n">
-        <v>25.24518775</v>
+        <v>29.811954</v>
       </c>
       <c r="AC37" t="n">
-        <v>25.163785</v>
+        <v>28.8289905</v>
       </c>
       <c r="AD37" t="n">
-        <v>20.5725872243042</v>
+        <v>6.56284659651471</v>
       </c>
       <c r="AE37" t="n">
         <v>4</v>
@@ -6428,52 +6401,52 @@
         <v>0.014514</v>
       </c>
       <c r="AG37" t="n">
-        <v>3.051471</v>
+        <v>0.09071</v>
       </c>
       <c r="AH37" t="n">
-        <v>1.0322755</v>
+        <v>0.044448</v>
       </c>
       <c r="AI37" t="n">
-        <v>0.5315585</v>
+        <v>0.036284</v>
       </c>
       <c r="AJ37" t="n">
-        <v>1.43167663903096</v>
+        <v>0.0370467479094544</v>
       </c>
       <c r="AK37" t="n">
         <v>4</v>
       </c>
       <c r="AL37" t="n">
-        <v>0.0990716962168577</v>
+        <v>0.0808756703113495</v>
       </c>
       <c r="AM37" t="n">
-        <v>0.648381916637629</v>
+        <v>1.15120732776973</v>
       </c>
       <c r="AN37" t="n">
-        <v>0.357429492797837</v>
+        <v>0.611734478996843</v>
       </c>
       <c r="AO37" t="n">
-        <v>0.341132179168432</v>
+        <v>0.607427458953147</v>
       </c>
       <c r="AP37" t="n">
-        <v>0.283950399338202</v>
+        <v>0.548302195244949</v>
       </c>
       <c r="AQ37" t="n">
         <v>4</v>
       </c>
       <c r="AR37" t="n">
-        <v>0.176915122211384</v>
+        <v>0.214061442351137</v>
       </c>
       <c r="AS37" t="n">
-        <v>3.79000022437559</v>
+        <v>2.25215131553443</v>
       </c>
       <c r="AT37" t="n">
-        <v>1.58654153424359</v>
+        <v>1.06061524543021</v>
       </c>
       <c r="AU37" t="n">
-        <v>1.1896253951937</v>
+        <v>0.888124111917628</v>
       </c>
       <c r="AV37" t="n">
-        <v>1.74035530741298</v>
+        <v>0.976836337978275</v>
       </c>
       <c r="AW37" t="n">
         <v>0</v>
@@ -6499,7 +6472,7 @@
         <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
         <v>56</v>
@@ -6508,148 +6481,148 @@
         <v>57</v>
       </c>
       <c r="G38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H38" t="n">
-        <v>1.766335786</v>
+        <v>0.3271206442</v>
       </c>
       <c r="I38" t="n">
-        <v>1.92280994</v>
+        <v>4.891769633</v>
       </c>
       <c r="J38" t="n">
-        <v>1.844572863</v>
+        <v>2.56107119705</v>
       </c>
       <c r="K38" t="n">
-        <v>1.844572863</v>
+        <v>2.5126972555</v>
       </c>
       <c r="L38" t="n">
-        <v>0.110643935373828</v>
+        <v>1.9704067798324</v>
       </c>
       <c r="M38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N38" t="n">
-        <v>0.002529152347</v>
+        <v>0.0002049663924</v>
       </c>
       <c r="O38" t="n">
-        <v>0.002819223341</v>
+        <v>0.006006712705</v>
       </c>
       <c r="P38" t="n">
-        <v>0.002674187844</v>
+        <v>0.00304728943185</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.002674187844</v>
+        <v>0.002988739315</v>
       </c>
       <c r="R38" t="n">
-        <v>0.000205111166882922</v>
+        <v>0.00255474362105596</v>
       </c>
       <c r="S38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T38" t="n">
-        <v>0.9989831778</v>
+        <v>0.987344213</v>
       </c>
       <c r="U38" t="n">
-        <v>0.9991156514</v>
+        <v>0.9985162009</v>
       </c>
       <c r="V38" t="n">
-        <v>0.9990494146</v>
+        <v>0.99477804315</v>
       </c>
       <c r="W38" t="n">
-        <v>0.9990494146</v>
+        <v>0.99662587935</v>
       </c>
       <c r="X38" t="n">
-        <v>0.0000936729808882055</v>
+        <v>0.0052561963832895</v>
       </c>
       <c r="Y38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z38" t="n">
-        <v>43.74263502</v>
+        <v>5.671158448</v>
       </c>
       <c r="AA38" t="n">
-        <v>44.6740719</v>
+        <v>52.35611571</v>
       </c>
       <c r="AB38" t="n">
-        <v>44.20835346</v>
+        <v>28.93355824175</v>
       </c>
       <c r="AC38" t="n">
-        <v>44.20835346</v>
+        <v>28.8534794045</v>
       </c>
       <c r="AD38" t="n">
-        <v>0.65862533409524</v>
+        <v>24.7612557834655</v>
       </c>
       <c r="AE38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AF38" t="n">
         <v>0.1004648173</v>
       </c>
       <c r="AG38" t="n">
-        <v>0.1004648173</v>
+        <v>9.899664123</v>
       </c>
       <c r="AH38" t="n">
-        <v>0.1004648173</v>
+        <v>3.0500100059</v>
       </c>
       <c r="AI38" t="n">
-        <v>0.1004648173</v>
+        <v>1.09995554165</v>
       </c>
       <c r="AJ38" t="n">
-        <v>0</v>
+        <v>4.66265184155628</v>
       </c>
       <c r="AK38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL38" t="n">
-        <v>0.07663489617</v>
+        <v>0.145071985</v>
       </c>
       <c r="AM38" t="n">
-        <v>0.09994383088</v>
+        <v>0.8618896844</v>
       </c>
       <c r="AN38" t="n">
-        <v>0.088289363525</v>
+        <v>0.4801019824</v>
       </c>
       <c r="AO38" t="n">
-        <v>0.088289363525</v>
+        <v>0.4567231301</v>
       </c>
       <c r="AP38" t="n">
-        <v>0.0164819057956755</v>
+        <v>0.384057841287175</v>
       </c>
       <c r="AQ38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AR38" t="n">
-        <v>0.2368160362</v>
+        <v>0.2414260519</v>
       </c>
       <c r="AS38" t="n">
-        <v>0.2608171702</v>
+        <v>3.567648922</v>
       </c>
       <c r="AT38" t="n">
-        <v>0.2488166032</v>
+        <v>1.41844556955</v>
       </c>
       <c r="AU38" t="n">
-        <v>0.2488166032</v>
+        <v>0.93235365215</v>
       </c>
       <c r="AV38" t="n">
-        <v>0.016971364607567</v>
+        <v>1.56491684526697</v>
       </c>
       <c r="AW38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AX38" t="n">
-        <v>0.01654115803</v>
+        <v>0.01698677161</v>
       </c>
       <c r="AY38" t="n">
-        <v>0.01702858706</v>
+        <v>0.02010935307</v>
       </c>
       <c r="AZ38" t="n">
-        <v>0.016784872545</v>
+        <v>0.01852792121</v>
       </c>
       <c r="BA38" t="n">
-        <v>0.016784872545</v>
+        <v>0.01850778008</v>
       </c>
       <c r="BB38" t="n">
-        <v>0.000344664372460181</v>
+        <v>0.00145825624227347</v>
       </c>
     </row>
     <row r="39">
@@ -6661,7 +6634,7 @@
         <v>74</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E39" t="s">
         <v>56</v>
@@ -6670,130 +6643,130 @@
         <v>58</v>
       </c>
       <c r="G39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H39" t="n">
-        <v>1.766335786</v>
+        <v>0.3271206442</v>
       </c>
       <c r="I39" t="n">
-        <v>1.92280994</v>
+        <v>4.891769633</v>
       </c>
       <c r="J39" t="n">
-        <v>1.844572863</v>
+        <v>2.56107119705</v>
       </c>
       <c r="K39" t="n">
-        <v>1.844572863</v>
+        <v>2.5126972555</v>
       </c>
       <c r="L39" t="n">
-        <v>0.110643935373828</v>
+        <v>1.9704067798324</v>
       </c>
       <c r="M39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N39" t="n">
-        <v>0.002211</v>
+        <v>0.000446</v>
       </c>
       <c r="O39" t="n">
-        <v>0.002693</v>
+        <v>0.005429</v>
       </c>
       <c r="P39" t="n">
-        <v>0.002452</v>
+        <v>0.00289075</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.002452</v>
+        <v>0.002844</v>
       </c>
       <c r="R39" t="n">
-        <v>0.000340825468531916</v>
+        <v>0.00226717436103475</v>
       </c>
       <c r="S39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T39" t="n">
-        <v>0.99972</v>
+        <v>0.995536</v>
       </c>
       <c r="U39" t="n">
-        <v>0.999842</v>
+        <v>0.999635</v>
       </c>
       <c r="V39" t="n">
-        <v>0.999781</v>
+        <v>0.99752775</v>
       </c>
       <c r="W39" t="n">
-        <v>0.999781</v>
+        <v>0.99747</v>
       </c>
       <c r="X39" t="n">
-        <v>0.0000862670273047273</v>
+        <v>0.00215654297043519</v>
       </c>
       <c r="Y39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z39" t="n">
-        <v>36.541066</v>
+        <v>5.658399</v>
       </c>
       <c r="AA39" t="n">
-        <v>37.182009</v>
+        <v>44.994782</v>
       </c>
       <c r="AB39" t="n">
-        <v>36.8615375</v>
+        <v>25.24518775</v>
       </c>
       <c r="AC39" t="n">
-        <v>36.8615375</v>
+        <v>25.163785</v>
       </c>
       <c r="AD39" t="n">
-        <v>0.453215141654049</v>
+        <v>20.5725872243042</v>
       </c>
       <c r="AE39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AF39" t="n">
         <v>0.014514</v>
       </c>
       <c r="AG39" t="n">
-        <v>0.014514</v>
+        <v>3.051471</v>
       </c>
       <c r="AH39" t="n">
-        <v>0.014514</v>
+        <v>1.0322755</v>
       </c>
       <c r="AI39" t="n">
-        <v>0.014514</v>
+        <v>0.5315585</v>
       </c>
       <c r="AJ39" t="n">
-        <v>0</v>
+        <v>1.43167663903096</v>
       </c>
       <c r="AK39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL39" t="n">
-        <v>0.0819297245978834</v>
+        <v>0.0990716962168577</v>
       </c>
       <c r="AM39" t="n">
-        <v>0.0880630245579665</v>
+        <v>0.648381916637629</v>
       </c>
       <c r="AN39" t="n">
-        <v>0.0849963745779249</v>
+        <v>0.357429492797837</v>
       </c>
       <c r="AO39" t="n">
-        <v>0.0849963745779249</v>
+        <v>0.341132179168432</v>
       </c>
       <c r="AP39" t="n">
-        <v>0.00433689799282594</v>
+        <v>0.283950399338202</v>
       </c>
       <c r="AQ39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AR39" t="n">
-        <v>0.167676762761206</v>
+        <v>0.176915122211384</v>
       </c>
       <c r="AS39" t="n">
-        <v>0.219674444929301</v>
+        <v>3.79000022437559</v>
       </c>
       <c r="AT39" t="n">
-        <v>0.193675603845254</v>
+        <v>1.58654153424359</v>
       </c>
       <c r="AU39" t="n">
-        <v>0.193675603845254</v>
+        <v>1.1896253951937</v>
       </c>
       <c r="AV39" t="n">
-        <v>0.0367679136670428</v>
+        <v>1.74035530741298</v>
       </c>
       <c r="AW39" t="n">
         <v>0</v>
@@ -6816,10 +6789,10 @@
       </c>
       <c r="B40"/>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E40" t="s">
         <v>56</v>
@@ -6828,148 +6801,148 @@
         <v>57</v>
       </c>
       <c r="G40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H40" t="n">
-        <v>0.2796867046</v>
+        <v>1.766335786</v>
       </c>
       <c r="I40" t="n">
-        <v>2.211462816</v>
+        <v>1.92280994</v>
       </c>
       <c r="J40" t="n">
-        <v>1.51740401353333</v>
+        <v>1.844572863</v>
       </c>
       <c r="K40" t="n">
-        <v>2.06106252</v>
+        <v>1.844572863</v>
       </c>
       <c r="L40" t="n">
-        <v>1.07452927595487</v>
+        <v>0.110643935373828</v>
       </c>
       <c r="M40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N40" t="n">
-        <v>0.001469931208</v>
+        <v>0.002529152347</v>
       </c>
       <c r="O40" t="n">
-        <v>0.004537845783</v>
+        <v>0.002819223341</v>
       </c>
       <c r="P40" t="n">
-        <v>0.00289722963233333</v>
+        <v>0.002674187844</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.002683911906</v>
+        <v>0.002674187844</v>
       </c>
       <c r="R40" t="n">
-        <v>0.00154504152020273</v>
+        <v>0.000205111166882922</v>
       </c>
       <c r="S40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T40" t="n">
-        <v>0.9971920728</v>
+        <v>0.9989831778</v>
       </c>
       <c r="U40" t="n">
-        <v>0.9992655104</v>
+        <v>0.9991156514</v>
       </c>
       <c r="V40" t="n">
-        <v>0.9983682546</v>
+        <v>0.9990494146</v>
       </c>
       <c r="W40" t="n">
-        <v>0.9986471806</v>
+        <v>0.9990494146</v>
       </c>
       <c r="X40" t="n">
-        <v>0.00106448844774401</v>
+        <v>0.0000936729808882055</v>
       </c>
       <c r="Y40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z40" t="n">
-        <v>4.795822322</v>
+        <v>43.74263502</v>
       </c>
       <c r="AA40" t="n">
-        <v>45.72611112</v>
+        <v>44.6740719</v>
       </c>
       <c r="AB40" t="n">
-        <v>31.0729556106667</v>
+        <v>44.20835346</v>
       </c>
       <c r="AC40" t="n">
-        <v>42.69693339</v>
+        <v>44.20835346</v>
       </c>
       <c r="AD40" t="n">
-        <v>22.8070116374931</v>
+        <v>0.65862533409524</v>
       </c>
       <c r="AE40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF40" t="n">
-        <v>0.08340500545</v>
+        <v>0.1004648173</v>
       </c>
       <c r="AG40" t="n">
         <v>0.1004648173</v>
       </c>
       <c r="AH40" t="n">
-        <v>0.09477821335</v>
+        <v>0.1004648173</v>
       </c>
       <c r="AI40" t="n">
         <v>0.1004648173</v>
       </c>
       <c r="AJ40" t="n">
-        <v>0.00984948696392186</v>
+        <v>0</v>
       </c>
       <c r="AK40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL40" t="n">
-        <v>0.0925234176</v>
+        <v>0.07663489617</v>
       </c>
       <c r="AM40" t="n">
-        <v>0.6360268217</v>
+        <v>0.09994383088</v>
       </c>
       <c r="AN40" t="n">
-        <v>0.298697730733333</v>
+        <v>0.088289363525</v>
       </c>
       <c r="AO40" t="n">
-        <v>0.1675429529</v>
+        <v>0.088289363525</v>
       </c>
       <c r="AP40" t="n">
-        <v>0.294533817037119</v>
+        <v>0.0164819057956755</v>
       </c>
       <c r="AQ40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR40" t="n">
-        <v>0.1887983624</v>
+        <v>0.2368160362</v>
       </c>
       <c r="AS40" t="n">
-        <v>1.683337179</v>
+        <v>0.2608171702</v>
       </c>
       <c r="AT40" t="n">
-        <v>0.696236755566667</v>
+        <v>0.2488166032</v>
       </c>
       <c r="AU40" t="n">
-        <v>0.2165747253</v>
+        <v>0.2488166032</v>
       </c>
       <c r="AV40" t="n">
-        <v>0.85496685084317</v>
+        <v>0.016971364607567</v>
       </c>
       <c r="AW40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AX40" t="n">
-        <v>0.01664714141</v>
+        <v>0.01654115803</v>
       </c>
       <c r="AY40" t="n">
-        <v>0.01736527476</v>
+        <v>0.01702858706</v>
       </c>
       <c r="AZ40" t="n">
-        <v>0.0170320436933333</v>
+        <v>0.016784872545</v>
       </c>
       <c r="BA40" t="n">
-        <v>0.01708371491</v>
+        <v>0.016784872545</v>
       </c>
       <c r="BB40" t="n">
-        <v>0.000361844321593439</v>
+        <v>0.000344664372460181</v>
       </c>
     </row>
     <row r="41">
@@ -6978,10 +6951,10 @@
       </c>
       <c r="B41"/>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" t="s">
         <v>56</v>
@@ -6990,130 +6963,130 @@
         <v>58</v>
       </c>
       <c r="G41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H41" t="n">
-        <v>0.2796867046</v>
+        <v>1.766335786</v>
       </c>
       <c r="I41" t="n">
-        <v>2.211462816</v>
+        <v>1.92280994</v>
       </c>
       <c r="J41" t="n">
-        <v>1.51740401353333</v>
+        <v>1.844572863</v>
       </c>
       <c r="K41" t="n">
-        <v>2.06106252</v>
+        <v>1.844572863</v>
       </c>
       <c r="L41" t="n">
-        <v>1.07452927595487</v>
+        <v>0.110643935373828</v>
       </c>
       <c r="M41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N41" t="n">
-        <v>0.001379</v>
+        <v>0.002211</v>
       </c>
       <c r="O41" t="n">
-        <v>0.006151</v>
+        <v>0.002693</v>
       </c>
       <c r="P41" t="n">
-        <v>0.00342733333333333</v>
+        <v>0.002452</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.002752</v>
+        <v>0.002452</v>
       </c>
       <c r="R41" t="n">
-        <v>0.00245663435075986</v>
+        <v>0.000340825468531916</v>
       </c>
       <c r="S41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T41" t="n">
-        <v>0.999316</v>
+        <v>0.99972</v>
       </c>
       <c r="U41" t="n">
-        <v>0.999841</v>
+        <v>0.999842</v>
       </c>
       <c r="V41" t="n">
-        <v>0.999665</v>
+        <v>0.999781</v>
       </c>
       <c r="W41" t="n">
-        <v>0.999838</v>
+        <v>0.999781</v>
       </c>
       <c r="X41" t="n">
-        <v>0.000302246588070078</v>
+        <v>0.0000862670273047273</v>
       </c>
       <c r="Y41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z41" t="n">
-        <v>4.104455</v>
+        <v>36.541066</v>
       </c>
       <c r="AA41" t="n">
-        <v>38.805949</v>
+        <v>37.182009</v>
       </c>
       <c r="AB41" t="n">
-        <v>26.3736316666667</v>
+        <v>36.8615375</v>
       </c>
       <c r="AC41" t="n">
-        <v>36.210491</v>
+        <v>36.8615375</v>
       </c>
       <c r="AD41" t="n">
-        <v>19.3292853622644</v>
+        <v>0.453215141654049</v>
       </c>
       <c r="AE41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF41" t="n">
         <v>0.014514</v>
       </c>
       <c r="AG41" t="n">
-        <v>0.032655</v>
+        <v>0.014514</v>
       </c>
       <c r="AH41" t="n">
-        <v>0.020561</v>
+        <v>0.014514</v>
       </c>
       <c r="AI41" t="n">
         <v>0.014514</v>
       </c>
       <c r="AJ41" t="n">
-        <v>0.010473711233369</v>
+        <v>0</v>
       </c>
       <c r="AK41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL41" t="n">
-        <v>0.0956187692539749</v>
+        <v>0.0819297245978834</v>
       </c>
       <c r="AM41" t="n">
-        <v>0.549041810844091</v>
+        <v>0.0880630245579665</v>
       </c>
       <c r="AN41" t="n">
-        <v>0.259380258861512</v>
+        <v>0.0849963745779249</v>
       </c>
       <c r="AO41" t="n">
-        <v>0.133480196486471</v>
+        <v>0.0849963745779249</v>
       </c>
       <c r="AP41" t="n">
-        <v>0.251567551446401</v>
+        <v>0.00433689799282594</v>
       </c>
       <c r="AQ41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR41" t="n">
-        <v>0.146022944367763</v>
+        <v>0.167676762761206</v>
       </c>
       <c r="AS41" t="n">
-        <v>1.59130841927121</v>
+        <v>0.219674444929301</v>
       </c>
       <c r="AT41" t="n">
-        <v>0.638286608932091</v>
+        <v>0.193675603845254</v>
       </c>
       <c r="AU41" t="n">
-        <v>0.177528463157301</v>
+        <v>0.193675603845254</v>
       </c>
       <c r="AV41" t="n">
-        <v>0.825491415863961</v>
+        <v>0.0367679136670428</v>
       </c>
       <c r="AW41" t="n">
         <v>0</v>
@@ -7136,145 +7109,161 @@
       </c>
       <c r="B42"/>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" t="s">
         <v>71</v>
-      </c>
-      <c r="E42" t="s">
-        <v>59</v>
       </c>
       <c r="F42" t="s">
         <v>57</v>
       </c>
       <c r="G42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H42" t="n">
-        <v>5.800245268</v>
+        <v>55.29409043</v>
       </c>
       <c r="I42" t="n">
-        <v>5.800245268</v>
+        <v>57.46477162</v>
       </c>
       <c r="J42" t="n">
-        <v>5.800245268</v>
+        <v>56.379431025</v>
       </c>
       <c r="K42" t="n">
-        <v>5.800245268</v>
-      </c>
-      <c r="L42"/>
+        <v>56.379431025</v>
+      </c>
+      <c r="L42" t="n">
+        <v>1.53490338924309</v>
+      </c>
       <c r="M42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N42" t="n">
-        <v>0.003140677635</v>
+        <v>0.005744431158</v>
       </c>
       <c r="O42" t="n">
-        <v>0.003140677635</v>
+        <v>0.006778044121</v>
       </c>
       <c r="P42" t="n">
-        <v>0.003140677635</v>
+        <v>0.0062612376395</v>
       </c>
       <c r="Q42" t="n">
-        <v>0.003140677635</v>
-      </c>
-      <c r="R42"/>
+        <v>0.0062612376395</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0.000730874735259621</v>
+      </c>
       <c r="S42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T42" t="n">
-        <v>0.9963200889</v>
+        <v>0.9770901387</v>
       </c>
       <c r="U42" t="n">
-        <v>0.9963200889</v>
+        <v>0.9868055389</v>
       </c>
       <c r="V42" t="n">
-        <v>0.9963200889</v>
+        <v>0.9819478388</v>
       </c>
       <c r="W42" t="n">
-        <v>0.9963200889</v>
-      </c>
-      <c r="X42"/>
+        <v>0.9819478388</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0.0068698253633611</v>
+      </c>
       <c r="Y42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z42" t="n">
-        <v>41.82057545</v>
+        <v>57.26896146</v>
       </c>
       <c r="AA42" t="n">
-        <v>41.82057545</v>
+        <v>60.77623934</v>
       </c>
       <c r="AB42" t="n">
-        <v>41.82057545</v>
+        <v>59.0226004</v>
       </c>
       <c r="AC42" t="n">
-        <v>41.82057545</v>
-      </c>
-      <c r="AD42"/>
+        <v>59.0226004</v>
+      </c>
+      <c r="AD42" t="n">
+        <v>2.48001997245358</v>
+      </c>
       <c r="AE42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF42" t="n">
-        <v>0.1868186706</v>
+        <v>0.03499639624</v>
       </c>
       <c r="AG42" t="n">
-        <v>0.1868186706</v>
+        <v>0.03723607985</v>
       </c>
       <c r="AH42" t="n">
-        <v>0.1868186706</v>
+        <v>0.036116238045</v>
       </c>
       <c r="AI42" t="n">
-        <v>0.1868186706</v>
-      </c>
-      <c r="AJ42"/>
+        <v>0.036116238045</v>
+      </c>
+      <c r="AJ42" t="n">
+        <v>0.00158369546834337</v>
+      </c>
       <c r="AK42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL42" t="n">
-        <v>0.4646806483</v>
+        <v>0.081692759</v>
       </c>
       <c r="AM42" t="n">
-        <v>0.4646806483</v>
+        <v>0.2011823972</v>
       </c>
       <c r="AN42" t="n">
-        <v>0.4646806483</v>
+        <v>0.1414375781</v>
       </c>
       <c r="AO42" t="n">
-        <v>0.4646806483</v>
-      </c>
-      <c r="AP42"/>
+        <v>0.1414375781</v>
+      </c>
+      <c r="AP42" t="n">
+        <v>0.0844919334527471</v>
+      </c>
       <c r="AQ42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR42" t="n">
-        <v>0.6964868487</v>
+        <v>0.2352776998</v>
       </c>
       <c r="AS42" t="n">
-        <v>0.6964868487</v>
+        <v>0.2521953865</v>
       </c>
       <c r="AT42" t="n">
-        <v>0.6964868487</v>
+        <v>0.24373654315</v>
       </c>
       <c r="AU42" t="n">
-        <v>0.6964868487</v>
-      </c>
-      <c r="AV42"/>
+        <v>0.24373654315</v>
+      </c>
+      <c r="AV42" t="n">
+        <v>0.0119626109875595</v>
+      </c>
       <c r="AW42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX42" t="n">
-        <v>0.01873237941</v>
+        <v>0.01544707514</v>
       </c>
       <c r="AY42" t="n">
-        <v>0.01873237941</v>
+        <v>0.02046846467</v>
       </c>
       <c r="AZ42" t="n">
-        <v>0.01873237941</v>
+        <v>0.017957769905</v>
       </c>
       <c r="BA42" t="n">
-        <v>0.01873237941</v>
-      </c>
-      <c r="BB42"/>
+        <v>0.017957769905</v>
+      </c>
+      <c r="BB42" t="n">
+        <v>0.00355065858764213</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
@@ -7282,129 +7271,143 @@
       </c>
       <c r="B43"/>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D43" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" t="s">
         <v>71</v>
-      </c>
-      <c r="E43" t="s">
-        <v>59</v>
       </c>
       <c r="F43" t="s">
         <v>58</v>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H43" t="n">
-        <v>5.800245268</v>
+        <v>55.29409043</v>
       </c>
       <c r="I43" t="n">
-        <v>5.800245268</v>
+        <v>57.46477162</v>
       </c>
       <c r="J43" t="n">
-        <v>5.800245268</v>
+        <v>56.379431025</v>
       </c>
       <c r="K43" t="n">
-        <v>5.800245268</v>
-      </c>
-      <c r="L43"/>
+        <v>56.379431025</v>
+      </c>
+      <c r="L43" t="n">
+        <v>1.53490338924309</v>
+      </c>
       <c r="M43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N43" t="n">
-        <v>0.002031</v>
+        <v>0.005426</v>
       </c>
       <c r="O43" t="n">
-        <v>0.002031</v>
+        <v>0.006865</v>
       </c>
       <c r="P43" t="n">
-        <v>0.002031</v>
+        <v>0.0061455</v>
       </c>
       <c r="Q43" t="n">
-        <v>0.002031</v>
-      </c>
-      <c r="R43"/>
+        <v>0.0061455</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0.00101752665812744</v>
+      </c>
       <c r="S43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T43" t="n">
-        <v>0.999047</v>
+        <v>0.981503</v>
       </c>
       <c r="U43" t="n">
-        <v>0.999047</v>
+        <v>0.98301</v>
       </c>
       <c r="V43" t="n">
-        <v>0.999047</v>
+        <v>0.9822565</v>
       </c>
       <c r="W43" t="n">
-        <v>0.999047</v>
-      </c>
-      <c r="X43"/>
+        <v>0.9822565</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0.00106560991924815</v>
+      </c>
       <c r="Y43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z43" t="n">
-        <v>34.331812</v>
+        <v>37.089792</v>
       </c>
       <c r="AA43" t="n">
-        <v>34.331812</v>
+        <v>37.643126</v>
       </c>
       <c r="AB43" t="n">
-        <v>34.331812</v>
+        <v>37.366459</v>
       </c>
       <c r="AC43" t="n">
-        <v>34.331812</v>
-      </c>
-      <c r="AD43"/>
+        <v>37.366459</v>
+      </c>
+      <c r="AD43" t="n">
+        <v>0.391266223661077</v>
+      </c>
       <c r="AE43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF43" t="n">
-        <v>0.032655</v>
+        <v>0.014514</v>
       </c>
       <c r="AG43" t="n">
-        <v>0.032655</v>
+        <v>0.014514</v>
       </c>
       <c r="AH43" t="n">
-        <v>0.032655</v>
+        <v>0.014514</v>
       </c>
       <c r="AI43" t="n">
-        <v>0.032655</v>
-      </c>
-      <c r="AJ43"/>
+        <v>0.014514</v>
+      </c>
+      <c r="AJ43" t="n">
+        <v>0</v>
+      </c>
       <c r="AK43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL43" t="n">
-        <v>0.226601855757112</v>
+        <v>0.102416813228951</v>
       </c>
       <c r="AM43" t="n">
-        <v>0.226601855757112</v>
+        <v>0.27295621724758</v>
       </c>
       <c r="AN43" t="n">
-        <v>0.226601855757112</v>
+        <v>0.187686515238266</v>
       </c>
       <c r="AO43" t="n">
-        <v>0.226601855757112</v>
-      </c>
-      <c r="AP43"/>
+        <v>0.187686515238266</v>
+      </c>
+      <c r="AP43" t="n">
+        <v>0.120589569041085</v>
+      </c>
       <c r="AQ43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR43" t="n">
-        <v>0.543975668752222</v>
+        <v>0.20086601338756</v>
       </c>
       <c r="AS43" t="n">
-        <v>0.543975668752222</v>
+        <v>0.297382541495459</v>
       </c>
       <c r="AT43" t="n">
-        <v>0.543975668752222</v>
+        <v>0.24912427744151</v>
       </c>
       <c r="AU43" t="n">
-        <v>0.543975668752222</v>
-      </c>
-      <c r="AV43"/>
+        <v>0.24912427744151</v>
+      </c>
+      <c r="AV43" t="n">
+        <v>0.0682474915216774</v>
+      </c>
       <c r="AW43" t="n">
         <v>0</v>
       </c>
@@ -7419,6 +7422,616 @@
       </c>
       <c r="BA43"/>
       <c r="BB43"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44"/>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44" t="n">
+        <v>3</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.2796867046</v>
+      </c>
+      <c r="I44" t="n">
+        <v>2.211462816</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1.51740401353333</v>
+      </c>
+      <c r="K44" t="n">
+        <v>2.06106252</v>
+      </c>
+      <c r="L44" t="n">
+        <v>1.07452927595487</v>
+      </c>
+      <c r="M44" t="n">
+        <v>3</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.001469931208</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.004537845783</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0.00289722963233333</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0.002683911906</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0.00154504152020273</v>
+      </c>
+      <c r="S44" t="n">
+        <v>3</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0.9971920728</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0.9992655104</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0.9983682546</v>
+      </c>
+      <c r="W44" t="n">
+        <v>0.9986471806</v>
+      </c>
+      <c r="X44" t="n">
+        <v>0.00106448844774401</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>4.795822322</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>45.72611112</v>
+      </c>
+      <c r="AB44" t="n">
+        <v>31.0729556106667</v>
+      </c>
+      <c r="AC44" t="n">
+        <v>42.69693339</v>
+      </c>
+      <c r="AD44" t="n">
+        <v>22.8070116374931</v>
+      </c>
+      <c r="AE44" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF44" t="n">
+        <v>0.08340500545</v>
+      </c>
+      <c r="AG44" t="n">
+        <v>0.1004648173</v>
+      </c>
+      <c r="AH44" t="n">
+        <v>0.09477821335</v>
+      </c>
+      <c r="AI44" t="n">
+        <v>0.1004648173</v>
+      </c>
+      <c r="AJ44" t="n">
+        <v>0.00984948696392186</v>
+      </c>
+      <c r="AK44" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL44" t="n">
+        <v>0.0925234176</v>
+      </c>
+      <c r="AM44" t="n">
+        <v>0.6360268217</v>
+      </c>
+      <c r="AN44" t="n">
+        <v>0.298697730733333</v>
+      </c>
+      <c r="AO44" t="n">
+        <v>0.1675429529</v>
+      </c>
+      <c r="AP44" t="n">
+        <v>0.294533817037119</v>
+      </c>
+      <c r="AQ44" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR44" t="n">
+        <v>0.1887983624</v>
+      </c>
+      <c r="AS44" t="n">
+        <v>1.683337179</v>
+      </c>
+      <c r="AT44" t="n">
+        <v>0.696236755566667</v>
+      </c>
+      <c r="AU44" t="n">
+        <v>0.2165747253</v>
+      </c>
+      <c r="AV44" t="n">
+        <v>0.85496685084317</v>
+      </c>
+      <c r="AW44" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX44" t="n">
+        <v>0.01664714141</v>
+      </c>
+      <c r="AY44" t="n">
+        <v>0.01736527476</v>
+      </c>
+      <c r="AZ44" t="n">
+        <v>0.0170320436933333</v>
+      </c>
+      <c r="BA44" t="n">
+        <v>0.01708371491</v>
+      </c>
+      <c r="BB44" t="n">
+        <v>0.000361844321593439</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45"/>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" t="s">
+        <v>58</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.2796867046</v>
+      </c>
+      <c r="I45" t="n">
+        <v>2.211462816</v>
+      </c>
+      <c r="J45" t="n">
+        <v>1.51740401353333</v>
+      </c>
+      <c r="K45" t="n">
+        <v>2.06106252</v>
+      </c>
+      <c r="L45" t="n">
+        <v>1.07452927595487</v>
+      </c>
+      <c r="M45" t="n">
+        <v>3</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.001379</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0.006151</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.00342733333333333</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0.002752</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0.00245663435075986</v>
+      </c>
+      <c r="S45" t="n">
+        <v>3</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0.999316</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0.999841</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0.999665</v>
+      </c>
+      <c r="W45" t="n">
+        <v>0.999838</v>
+      </c>
+      <c r="X45" t="n">
+        <v>0.000302246588070078</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>4.104455</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>38.805949</v>
+      </c>
+      <c r="AB45" t="n">
+        <v>26.3736316666667</v>
+      </c>
+      <c r="AC45" t="n">
+        <v>36.210491</v>
+      </c>
+      <c r="AD45" t="n">
+        <v>19.3292853622644</v>
+      </c>
+      <c r="AE45" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF45" t="n">
+        <v>0.014514</v>
+      </c>
+      <c r="AG45" t="n">
+        <v>0.032655</v>
+      </c>
+      <c r="AH45" t="n">
+        <v>0.020561</v>
+      </c>
+      <c r="AI45" t="n">
+        <v>0.014514</v>
+      </c>
+      <c r="AJ45" t="n">
+        <v>0.010473711233369</v>
+      </c>
+      <c r="AK45" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL45" t="n">
+        <v>0.0956187692539749</v>
+      </c>
+      <c r="AM45" t="n">
+        <v>0.549041810844091</v>
+      </c>
+      <c r="AN45" t="n">
+        <v>0.259380258861512</v>
+      </c>
+      <c r="AO45" t="n">
+        <v>0.133480196486471</v>
+      </c>
+      <c r="AP45" t="n">
+        <v>0.251567551446401</v>
+      </c>
+      <c r="AQ45" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR45" t="n">
+        <v>0.146022944367763</v>
+      </c>
+      <c r="AS45" t="n">
+        <v>1.59130841927121</v>
+      </c>
+      <c r="AT45" t="n">
+        <v>0.638286608932091</v>
+      </c>
+      <c r="AU45" t="n">
+        <v>0.177528463157301</v>
+      </c>
+      <c r="AV45" t="n">
+        <v>0.825491415863961</v>
+      </c>
+      <c r="AW45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX45" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AY45" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AZ45" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="BA45"/>
+      <c r="BB45"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46"/>
+      <c r="C46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" t="s">
+        <v>57</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="I46" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="J46" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="K46" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="L46"/>
+      <c r="M46" t="n">
+        <v>1</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.003140677635</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0.003140677635</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.003140677635</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0.003140677635</v>
+      </c>
+      <c r="R46"/>
+      <c r="S46" t="n">
+        <v>1</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0.9963200889</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0.9963200889</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0.9963200889</v>
+      </c>
+      <c r="W46" t="n">
+        <v>0.9963200889</v>
+      </c>
+      <c r="X46"/>
+      <c r="Y46" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>41.82057545</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>41.82057545</v>
+      </c>
+      <c r="AB46" t="n">
+        <v>41.82057545</v>
+      </c>
+      <c r="AC46" t="n">
+        <v>41.82057545</v>
+      </c>
+      <c r="AD46"/>
+      <c r="AE46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF46" t="n">
+        <v>0.1868186706</v>
+      </c>
+      <c r="AG46" t="n">
+        <v>0.1868186706</v>
+      </c>
+      <c r="AH46" t="n">
+        <v>0.1868186706</v>
+      </c>
+      <c r="AI46" t="n">
+        <v>0.1868186706</v>
+      </c>
+      <c r="AJ46"/>
+      <c r="AK46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL46" t="n">
+        <v>0.4646806483</v>
+      </c>
+      <c r="AM46" t="n">
+        <v>0.4646806483</v>
+      </c>
+      <c r="AN46" t="n">
+        <v>0.4646806483</v>
+      </c>
+      <c r="AO46" t="n">
+        <v>0.4646806483</v>
+      </c>
+      <c r="AP46"/>
+      <c r="AQ46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR46" t="n">
+        <v>0.6964868487</v>
+      </c>
+      <c r="AS46" t="n">
+        <v>0.6964868487</v>
+      </c>
+      <c r="AT46" t="n">
+        <v>0.6964868487</v>
+      </c>
+      <c r="AU46" t="n">
+        <v>0.6964868487</v>
+      </c>
+      <c r="AV46"/>
+      <c r="AW46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX46" t="n">
+        <v>0.01873237941</v>
+      </c>
+      <c r="AY46" t="n">
+        <v>0.01873237941</v>
+      </c>
+      <c r="AZ46" t="n">
+        <v>0.01873237941</v>
+      </c>
+      <c r="BA46" t="n">
+        <v>0.01873237941</v>
+      </c>
+      <c r="BB46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47"/>
+      <c r="C47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="I47" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="J47" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="K47" t="n">
+        <v>5.800245268</v>
+      </c>
+      <c r="L47"/>
+      <c r="M47" t="n">
+        <v>1</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.002031</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.002031</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0.002031</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0.002031</v>
+      </c>
+      <c r="R47"/>
+      <c r="S47" t="n">
+        <v>1</v>
+      </c>
+      <c r="T47" t="n">
+        <v>0.999047</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0.999047</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0.999047</v>
+      </c>
+      <c r="W47" t="n">
+        <v>0.999047</v>
+      </c>
+      <c r="X47"/>
+      <c r="Y47" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>34.331812</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>34.331812</v>
+      </c>
+      <c r="AB47" t="n">
+        <v>34.331812</v>
+      </c>
+      <c r="AC47" t="n">
+        <v>34.331812</v>
+      </c>
+      <c r="AD47"/>
+      <c r="AE47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF47" t="n">
+        <v>0.032655</v>
+      </c>
+      <c r="AG47" t="n">
+        <v>0.032655</v>
+      </c>
+      <c r="AH47" t="n">
+        <v>0.032655</v>
+      </c>
+      <c r="AI47" t="n">
+        <v>0.032655</v>
+      </c>
+      <c r="AJ47"/>
+      <c r="AK47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL47" t="n">
+        <v>0.226601855757112</v>
+      </c>
+      <c r="AM47" t="n">
+        <v>0.226601855757112</v>
+      </c>
+      <c r="AN47" t="n">
+        <v>0.226601855757112</v>
+      </c>
+      <c r="AO47" t="n">
+        <v>0.226601855757112</v>
+      </c>
+      <c r="AP47"/>
+      <c r="AQ47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR47" t="n">
+        <v>0.543975668752222</v>
+      </c>
+      <c r="AS47" t="n">
+        <v>0.543975668752222</v>
+      </c>
+      <c r="AT47" t="n">
+        <v>0.543975668752222</v>
+      </c>
+      <c r="AU47" t="n">
+        <v>0.543975668752222</v>
+      </c>
+      <c r="AV47"/>
+      <c r="AW47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX47" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AY47" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AZ47" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="BA47"/>
+      <c r="BB47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7436,82 +8049,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>